<commit_message>
Se corrigio  el limpiador para que funcione en bloques o completo,queda cambiar para que funcione de mas de 2
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Informes/Excel/6.xlsx
+++ b/Archivos de trabajo/Informes/Excel/6.xlsx
@@ -557,10 +557,10 @@
         <v>44106</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>44106.27291666667</v>
+        <v>44106</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>44106.70069444443</v>
+        <v>44106</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>44106</v>
@@ -588,7 +588,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Otro</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -597,10 +597,10 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>1.43</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -691,10 +691,10 @@
         <v>44110</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>44110.27361111111</v>
+        <v>44110</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>44110.70069444443</v>
+        <v>44110</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>44110</v>
@@ -722,19 +722,19 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Enfermedad</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Colera</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>1.42</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>7.98</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1093,7 +1093,7 @@
         <v>44118</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>44118.27152777778</v>
+        <v>44118.33472222222</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>44118.70208333333</v>
@@ -1133,10 +1133,10 @@
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>8</v>
+        <v>7.97</v>
       </c>
       <c r="R10" t="n">
-        <v>1.5</v>
+        <v>0.03</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1270,10 +1270,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>72</v>
+        <v>55.97</v>
       </c>
       <c r="D2" t="n">
-        <v>21.48</v>
+        <v>9.18</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>

</xml_diff>